<commit_message>
Updated user stories based on feedback from Discord
</commit_message>
<xml_diff>
--- a/CS482-Triangle-GoFish-Requirements-Revised.xlsx
+++ b/CS482-Triangle-GoFish-Requirements-Revised.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B435F8D2-9760-4385-B889-E0F9A692CBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41B69BC-EB09-4845-8E8E-E48B339B6232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5988" yWindow="0" windowWidth="17184" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -622,7 +622,7 @@
     <t>Game Flow</t>
   </si>
   <si>
-    <t xml:space="preserve">Essential for playing the actual card game of Go Fish. </t>
+    <t xml:space="preserve">Essential stories for the experience playing the actual card game of Go Fish. </t>
   </si>
 </sst>
 </file>
@@ -755,7 +755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -806,7 +806,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1148,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X1000"/>
+  <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="113" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1273,7 +1272,7 @@
         <v>27</v>
       </c>
       <c r="K3" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4" t="s">
@@ -1312,7 +1311,7 @@
         <v>32</v>
       </c>
       <c r="K4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
@@ -1351,7 +1350,7 @@
         <v>38</v>
       </c>
       <c r="K5" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="10"/>
       <c r="M5" s="10" t="s">
@@ -1435,7 +1434,7 @@
         <v>44</v>
       </c>
       <c r="K9" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L9" s="22"/>
       <c r="M9" s="10" t="s">
@@ -1472,7 +1471,7 @@
         <v>50</v>
       </c>
       <c r="K10" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" s="22"/>
       <c r="M10" s="10" t="s">
@@ -1509,7 +1508,7 @@
         <v>55</v>
       </c>
       <c r="K11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="22"/>
       <c r="M11" s="10" t="s">
@@ -1548,7 +1547,7 @@
         <v>60</v>
       </c>
       <c r="K12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="10" t="s">
@@ -1587,7 +1586,7 @@
         <v>65</v>
       </c>
       <c r="K13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="10" t="s">
@@ -1626,7 +1625,7 @@
         <v>71</v>
       </c>
       <c r="K14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="10" t="s">
@@ -1665,7 +1664,7 @@
         <v>76</v>
       </c>
       <c r="K15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="10" t="s">
@@ -1704,7 +1703,7 @@
         <v>82</v>
       </c>
       <c r="K16" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="10" t="s">
@@ -1743,7 +1742,7 @@
         <v>87</v>
       </c>
       <c r="K17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="10" t="s">
@@ -1782,7 +1781,7 @@
         <v>92</v>
       </c>
       <c r="K18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="10" t="s">
@@ -1821,7 +1820,7 @@
         <v>97</v>
       </c>
       <c r="K19" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
@@ -1899,7 +1898,7 @@
         <v>108</v>
       </c>
       <c r="K21" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="10" t="s">
@@ -1938,7 +1937,7 @@
         <v>113</v>
       </c>
       <c r="K22" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="10" t="s">
@@ -1977,7 +1976,7 @@
         <v>118</v>
       </c>
       <c r="K23" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="10" t="s">
@@ -2016,7 +2015,7 @@
         <v>123</v>
       </c>
       <c r="K24" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L24" s="5"/>
       <c r="M24" s="10" t="s">
@@ -2058,7 +2057,7 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="26" t="s">
         <v>124</v>
       </c>
       <c r="F27" s="23"/>
@@ -2207,7 +2206,7 @@
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="26" t="s">
         <v>144</v>
       </c>
       <c r="F32" s="5"/>
@@ -2221,7 +2220,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>145</v>
       </c>
@@ -2253,14 +2252,14 @@
         <v>151</v>
       </c>
       <c r="K33" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L33" s="10"/>
       <c r="M33" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>152</v>
       </c>
@@ -2292,14 +2291,14 @@
         <v>156</v>
       </c>
       <c r="K34" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L34" s="10"/>
       <c r="M34" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>157</v>
       </c>
@@ -2331,14 +2330,14 @@
         <v>161</v>
       </c>
       <c r="K35" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L35" s="10"/>
       <c r="M35" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>162</v>
       </c>
@@ -2370,23 +2369,14 @@
         <v>166</v>
       </c>
       <c r="K36" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L36" s="10"/>
       <c r="M36" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="N36" s="24"/>
-      <c r="O36" s="24"/>
-      <c r="P36" s="24"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24"/>
-      <c r="S36" s="24"/>
-      <c r="T36" s="24"/>
-      <c r="U36" s="24"/>
-      <c r="V36" s="24"/>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>167</v>
       </c>
@@ -2424,34 +2414,25 @@
       <c r="M37" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="N37" s="24"/>
-      <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="24"/>
-      <c r="R37" s="24"/>
-      <c r="S37" s="24"/>
-      <c r="T37" s="24"/>
-      <c r="U37" s="24"/>
-      <c r="V37" s="24"/>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
     </row>
-    <row r="40" spans="1:24" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="40" spans="1:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A40" s="10"/>
       <c r="B40" s="13" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="10"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="18"/>
       <c r="C42" s="11" t="s">
@@ -2462,7 +2443,7 @@
       <c r="F42" s="11"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="10"/>
       <c r="B43" s="19"/>
       <c r="C43" s="11" t="s">
@@ -2472,7 +2453,7 @@
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
       <c r="B44" s="20"/>
       <c r="C44" s="11" t="s">
@@ -2482,7 +2463,7 @@
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>
       <c r="B45" s="21"/>
       <c r="C45" s="11" t="s">
@@ -2492,10 +2473,10 @@
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="10"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="9"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -2509,67 +2490,53 @@
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B48" s="25" t="s">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B48" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="26"/>
-      <c r="N48" s="25"/>
-      <c r="O48" s="24"/>
-      <c r="P48" s="24"/>
-      <c r="Q48" s="24"/>
-      <c r="R48" s="24"/>
-      <c r="S48" s="24"/>
-      <c r="T48" s="24"/>
-      <c r="U48" s="24"/>
-      <c r="V48" s="24"/>
-      <c r="W48" s="24"/>
-      <c r="X48" s="24"/>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
+      <c r="K48" s="24"/>
+      <c r="L48" s="24"/>
+      <c r="M48" s="25"/>
+      <c r="N48" s="24"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="10"/>
-      <c r="B49" s="25" t="s">
+      <c r="B49" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="25"/>
-      <c r="N49" s="25"/>
-      <c r="O49" s="25"/>
-      <c r="P49" s="25"/>
-      <c r="Q49" s="25"/>
-      <c r="R49" s="25"/>
-      <c r="S49" s="25"/>
-      <c r="T49" s="25"/>
-      <c r="U49" s="25"/>
-      <c r="V49" s="24"/>
-      <c r="W49" s="24"/>
-      <c r="X49" s="24"/>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24"/>
+      <c r="K49" s="24"/>
+      <c r="L49" s="24"/>
+      <c r="M49" s="24"/>
+      <c r="N49" s="24"/>
+      <c r="O49" s="24"/>
+      <c r="P49" s="24"/>
+      <c r="Q49" s="24"/>
+      <c r="R49" s="24"/>
+      <c r="S49" s="24"/>
+      <c r="T49" s="24"/>
+      <c r="U49" s="24"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="10"/>
       <c r="L50" s="4"/>
-      <c r="M50" s="24"/>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="10"/>
       <c r="B51" s="4" t="s">
         <v>179</v>
@@ -2586,7 +2553,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="8" t="s">
         <v>180</v>
@@ -2621,41 +2588,41 @@
       <c r="L52" s="10"/>
       <c r="M52" s="4"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="M53" s="10"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>